<commit_message>
CSC Assessment memorial Day
</commit_message>
<xml_diff>
--- a/2020-2021/CSC4350 Writing Initiative.xlsx
+++ b/2020-2021/CSC4350 Writing Initiative.xlsx
@@ -504,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,8 +559,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1">
-        <f>95/100</f>
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="E3" s="7">
         <f>38.4/40</f>
@@ -580,8 +579,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <f>82.5/100</f>
-        <v>0.82499999999999996</v>
+        <v>82</v>
       </c>
       <c r="E4">
         <f>34/40</f>
@@ -658,8 +656,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <f>78/100</f>
-        <v>0.78</v>
+        <v>78</v>
       </c>
       <c r="E8">
         <f>30/40</f>
@@ -1061,7 +1058,7 @@
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <f>AVERAGE(D3:D28)</f>
-        <v>75.679038461538468</v>
+        <v>85.388461538461542</v>
       </c>
       <c r="E29" s="1">
         <f>AVERAGE(E3:E27)</f>
@@ -1074,6 +1071,24 @@
       <c r="G29" s="1">
         <f>AVERAGE(G3:G27)</f>
         <v>0.83007346666666659</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
+        <f>5*0.85</f>
+        <v>4.25</v>
+      </c>
+      <c r="E30">
+        <f>5*E29</f>
+        <v>4.1449999999999996</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ref="F30:G30" si="0">5*F29</f>
+        <v>4.2100000000000009</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>4.1503673333333326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>